<commit_message>
add SMOTE & new dataset
</commit_message>
<xml_diff>
--- a/data_set2 (1).xlsx
+++ b/data_set2 (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tegar\7. Tegar\Skrispi\Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tegar\7. Tegar\Skrispi\Skripsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0C1E5D-1CA8-4252-B1EA-70780D06BA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71362262-FF3C-467F-AAE2-58AA52440D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4135" uniqueCount="1714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="1716">
   <si>
     <t>IDJwb</t>
   </si>
@@ -5233,6 +5233,12 @@
   </si>
   <si>
     <t>Elemen Dasar : Assets : berisi penyimpanan files; Structure : berisi tentang informasi arsitektur file nya; Services : sarana untuk mengakses assets, misalnya pelayanan atau; jaringan; Display : dalam display assets harus diatur menggunakan informasi arsitektur untuk ditampilkan melaluii kompleks jasa. Contoh : Disini saya mengambil contoh digitalizing Baju adat Indonesia. Rancangan : Mengscan object nya , kemudian mengecek kualitas (hasil scan) dengan yang asli jika sudah cukup / tidak ada yang kurang bisa langsung di di simpan / digunakan , biasanya scan akan menghasilkan sedikit kecacatan texture, jika terjadi maka harus di benarkan (biasanya menggunakan VX Model / Autodesk Mudbox (Tergantung masalahnya) ); Assets : Keseluruhan baju adat nya ( textur baju nya, motif bajunya , aksesoris yang digunakan , bahan ?); Services : 3-D Model dari baju adat; Meta data : Deskriptif , Terbuat dari kain apa , asal daerahnya, digunakan untuk acara apa saja, aksesoris tambahan; Tools : 3-D Camera Scanner (Metrology-Grade 3D Scanner , Professional-; Grade 3D Scanner , dll), software untuk melakukan repair texture yang cacat (VX Model, Autodesk Mudbox), seperangkat computer (mid – high end), Baju adatnya , lighting. Alasan memilih : Baju adat : karena harus melesatarikan budaya sendiri , karena pakaian adat sudah mulai menghilang karena banyaknya trend trend negara lain yang masuk ke Indonesia sehingga adat adat tradisional mulai; hilang; Tool : karena memang itu yang dibutuhkan; Data Form : karena 3-D Model merupakan presentasi yang paling tepat menurut kelompok kami karena pakaian adat memiliki banyak detail detail yang penting (aksesoris yang dipakai , dll) “Laser Scanning” / “White Light body scanning” (metode nya ).</t>
+  </si>
+  <si>
+    <t>Jumlah Soal Stelma</t>
+  </si>
+  <si>
+    <t>Jumlah Soal UKDW</t>
   </si>
 </sst>
 </file>
@@ -5708,8 +5714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1057"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -6053,7 +6059,7 @@
         <v>42</v>
       </c>
       <c r="O6" s="14">
-        <f>COUNTIF($I$102:$I$143,"A")</f>
+        <f>COUNTIF($I$103:$I$143,"A")</f>
         <v>5</v>
       </c>
       <c r="P6" s="17">
@@ -6089,11 +6095,11 @@
         <v>40</v>
       </c>
       <c r="X6" s="14">
-        <f>COUNTIF($I$664:$I$784,"A")</f>
+        <f>COUNTIF($I$664:$I$783,"A")</f>
         <v>22</v>
       </c>
       <c r="Y6" s="14">
-        <f>COUNTIF($I$785:$I$818,"A")</f>
+        <f>COUNTIF($I$784:$I$818,"A")</f>
         <v>5</v>
       </c>
       <c r="Z6" s="14"/>
@@ -6145,7 +6151,7 @@
         <v>14</v>
       </c>
       <c r="O7" s="14">
-        <f>COUNTIF($I$102:$I$143,"B")</f>
+        <f>COUNTIF($I$103:$I$143,"B")</f>
         <v>10</v>
       </c>
       <c r="P7" s="17">
@@ -6181,11 +6187,11 @@
         <v>41</v>
       </c>
       <c r="X7" s="14">
-        <f>COUNTIF($I$664:$I$784,"B")</f>
+        <f>COUNTIF($I$664:$I$783,"B")</f>
         <v>10</v>
       </c>
       <c r="Y7" s="14">
-        <f>COUNTIF($I$785:$I$818,"B")</f>
+        <f>COUNTIF($I$784:$I$818,"B")</f>
         <v>6</v>
       </c>
       <c r="Z7" s="14"/>
@@ -6237,7 +6243,7 @@
         <v>25</v>
       </c>
       <c r="O8" s="14">
-        <f>COUNTIF($I$102:$I$143,"C")</f>
+        <f>COUNTIF($I$103:$I$143,"C")</f>
         <v>5</v>
       </c>
       <c r="P8" s="17">
@@ -6273,12 +6279,12 @@
         <v>10</v>
       </c>
       <c r="X8" s="14">
-        <f>COUNTIF($I$664:$I$784,"C")</f>
+        <f>COUNTIF($I$664:$I$783,"C")</f>
+        <v>13</v>
+      </c>
+      <c r="Y8" s="14">
+        <f>COUNTIF($I$784:$I$818,"C")</f>
         <v>14</v>
-      </c>
-      <c r="Y8" s="14">
-        <f>COUNTIF($I$785:$I$818,"C")</f>
-        <v>13</v>
       </c>
       <c r="Z8" s="14"/>
     </row>
@@ -6329,8 +6335,8 @@
         <v>10</v>
       </c>
       <c r="O9" s="14">
-        <f>COUNTIF($I$102:$I$143,"D")</f>
-        <v>6</v>
+        <f>COUNTIF($I$103:$I$143,"D")</f>
+        <v>5</v>
       </c>
       <c r="P9" s="17">
         <f>COUNTIF($I$144:$I$176,"D")</f>
@@ -6365,11 +6371,11 @@
         <v>10</v>
       </c>
       <c r="X9" s="14">
-        <f>COUNTIF($I$664:$I$784,"D")</f>
+        <f>COUNTIF($I$664:$I$783,"D")</f>
         <v>10</v>
       </c>
       <c r="Y9" s="14">
-        <f>COUNTIF($I$785:$I$818,"D")</f>
+        <f>COUNTIF($I$784:$I$818,"D")</f>
         <v>5</v>
       </c>
       <c r="Z9" s="14"/>
@@ -6417,11 +6423,11 @@
         <v>213</v>
       </c>
       <c r="N10" s="14">
-        <f>COUNTIF($I$2:$I$102,"A")</f>
-        <v>42</v>
+        <f>COUNTIF($I$2:$I$102,"E")</f>
+        <v>10</v>
       </c>
       <c r="O10" s="14">
-        <f>COUNTIF($I$102:$I$143,"E")</f>
+        <f>COUNTIF($I$103:$I$143,"E")</f>
         <v>16</v>
       </c>
       <c r="P10" s="17">
@@ -6457,11 +6463,11 @@
         <v>13</v>
       </c>
       <c r="X10" s="14">
-        <f>COUNTIF($I$664:$I$784,"E")</f>
+        <f>COUNTIF($I$664:$I$783,"E")</f>
         <v>65</v>
       </c>
       <c r="Y10" s="14">
-        <f>COUNTIF($I$785:$I$818,"E")</f>
+        <f>COUNTIF($I$784:$I$818,"E")</f>
         <v>5</v>
       </c>
       <c r="Z10" s="14"/>
@@ -6510,11 +6516,11 @@
       </c>
       <c r="N11" s="16">
         <f t="shared" si="3"/>
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="O11" s="16">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P11" s="16">
         <f t="shared" si="3"/>
@@ -6550,11 +6556,11 @@
       </c>
       <c r="X11" s="16">
         <f t="shared" si="3"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y11" s="16">
         <f t="shared" si="3"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z11" s="14"/>
     </row>
@@ -6644,8 +6650,13 @@
         <v>5</v>
       </c>
       <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
+      <c r="L13" s="14" t="s">
+        <v>1714</v>
+      </c>
+      <c r="M13" s="14">
+        <f>SUM(N11,U11,V11,W11,X11)</f>
+        <v>550</v>
+      </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -6695,8 +6706,13 @@
         <v>2</v>
       </c>
       <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
+      <c r="L14" s="14" t="s">
+        <v>1715</v>
+      </c>
+      <c r="M14" s="14">
+        <f>SUM(O11:T11,Y11)</f>
+        <v>267</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>

</xml_diff>